<commit_message>
forms, read file, documents, traits revision, fix unautAccess, css
</commit_message>
<xml_diff>
--- a/documentation/Sprint Burndown Chart.xlsx
+++ b/documentation/Sprint Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Donkerdom\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55B0BDF-5B0B-4E46-B5AC-B1CAF0570D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B77A4A2-12E2-4CEB-ABC4-C8682AD86AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F612ECB5-40F1-4613-AC34-6EB1D630DFD2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>PDO (PHP)</t>
+  </si>
+  <si>
+    <t>Update(PHP)</t>
+  </si>
+  <si>
+    <t>Delete(PHP)</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +193,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -301,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,10 +322,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,37 +355,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -530,16 +546,16 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,7 +1769,7 @@
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,72 +1783,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="9">
         <v>45390</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="9">
         <v>45391</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="10">
         <v>45392</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="10">
         <v>45393</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="10">
         <v>45394</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="15" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1843,11 +1859,13 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="11">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1859,11 +1877,13 @@
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="11">
         <v>2</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1875,14 +1895,18 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="11">
         <v>4</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
@@ -1893,11 +1917,13 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="11">
         <v>2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1909,11 +1935,13 @@
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="11">
         <v>2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1925,11 +1953,13 @@
       <c r="C11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="11">
         <v>2</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1941,13 +1971,15 @@
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="11">
         <v>2</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1955,7 +1987,7 @@
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="19">
+      <c r="D13" s="11">
         <v>2</v>
       </c>
       <c r="E13" s="1"/>
@@ -1967,7 +1999,7 @@
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="19">
+      <c r="D14" s="11">
         <v>2</v>
       </c>
       <c r="E14" s="1"/>
@@ -1977,177 +2009,185 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
+      <c r="B15" s="21">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="19">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>2</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="D15" s="22">
+        <v>2</v>
+      </c>
+      <c r="E15" s="22">
+        <v>2</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
+      <c r="B16" s="21">
         <v>10</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="19">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="D16" s="22">
+        <v>2</v>
+      </c>
+      <c r="E16" s="22">
+        <v>2</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
+      <c r="B17" s="21">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="19">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="D17" s="22">
+        <v>2</v>
+      </c>
+      <c r="E17" s="22">
+        <v>2</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
+      <c r="B18" s="21">
         <v>10</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="19">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="D18" s="22">
+        <v>2</v>
+      </c>
+      <c r="E18" s="22">
+        <v>2</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
+      <c r="B19" s="21">
         <v>11</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="22">
         <v>1</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="22">
         <v>1</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
+      <c r="B20" s="21">
         <v>12</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="19">
-        <v>2</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="D20" s="22">
+        <v>2</v>
+      </c>
+      <c r="E20" s="22">
+        <v>2</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
+      <c r="B21" s="21">
         <v>13</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="22">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="22">
         <v>1</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
+      <c r="B22" s="21">
         <v>16</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="19">
-        <v>2</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="D22" s="22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="19">
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="11">
         <v>2</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="19">
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="11">
         <v>2</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="20">
+      <c r="D25" s="12">
         <v>2</v>
       </c>
       <c r="E25" s="3"/>
@@ -2157,61 +2197,61 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12">
+      <c r="C26" s="14"/>
+      <c r="D26" s="6">
         <f>SUM(D6:D25)</f>
         <v>40</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="7">
         <f>D26-SUM(E6:E25)</f>
         <v>24</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="7">
         <f t="shared" ref="F26:I26" si="0">E26-SUM(F6:F25)</f>
-        <v>24</v>
-      </c>
-      <c r="G26" s="13">
+        <v>17</v>
+      </c>
+      <c r="G26" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="H26" s="13">
+        <v>14</v>
+      </c>
+      <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="I26" s="13">
+        <v>14</v>
+      </c>
+      <c r="I26" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8">
+      <c r="C27" s="16"/>
+      <c r="D27" s="4">
         <f>SUM(D6:D25)</f>
         <v>40</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="5">
         <f>$D$27-($D$27/5*1)</f>
         <v>32</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="5">
         <f>$D$27-($D$27/5*2)</f>
         <v>24</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="5">
         <f>$D$27-($D$27/5*3)</f>
         <v>16</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="5">
         <f>$D$27-($D$27/5*4)</f>
         <v>8</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="5">
         <f>$D$27-($D$27/5*5)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
code cleanup, update, delete, reads, filter, css
</commit_message>
<xml_diff>
--- a/documentation/Sprint Burndown Chart.xlsx
+++ b/documentation/Sprint Burndown Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Donkerdom\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B77A4A2-12E2-4CEB-ABC4-C8682AD86AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C00DD5-CE13-4A59-9515-69B5D494F594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F612ECB5-40F1-4613-AC34-6EB1D630DFD2}"/>
+    <workbookView xWindow="1740" yWindow="1536" windowWidth="18588" windowHeight="10704" xr2:uid="{F612ECB5-40F1-4613-AC34-6EB1D630DFD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Informatie Tabel</t>
   </si>
   <si>
-    <t>Filters Tabel</t>
-  </si>
-  <si>
     <t>Homepage</t>
   </si>
   <si>
@@ -123,6 +120,18 @@
   </si>
   <si>
     <t>Delete(PHP)</t>
+  </si>
+  <si>
+    <t>Read (PHP)</t>
+  </si>
+  <si>
+    <t>overige documenten</t>
+  </si>
+  <si>
+    <t>Stem-systeem</t>
+  </si>
+  <si>
+    <t>Filter Knop Tabel</t>
   </si>
 </sst>
 </file>
@@ -313,15 +322,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,7 +346,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,10 +382,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,22 +552,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -635,19 +647,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>25.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>16.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>8.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1768,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9937272-FC32-427D-8DD5-1BBD654D3D76}">
   <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,201 +1795,213 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>45390</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>45391</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>45392</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>45393</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>45394</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="D6" s="12">
+        <v>2</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="D7" s="12">
+        <v>2</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1"/>
+      <c r="E8" s="12">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <v>1</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
+      <c r="B9" s="11">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="11">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="D9" s="12">
+        <v>2</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+      <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1"/>
+      <c r="D10" s="12">
+        <v>2</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
+      <c r="B11" s="11">
         <v>6</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="11">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="11">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="D12" s="12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12">
         <v>1</v>
       </c>
       <c r="G12" s="1"/>
@@ -1986,20 +2010,28 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="11">
-        <v>2</v>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="10">
+        <v>4</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="11">
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="10">
         <v>2</v>
       </c>
       <c r="E14" s="1"/>
@@ -2009,249 +2041,263 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="21">
+      <c r="B15" s="11">
         <v>10</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" s="12">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="11">
+        <v>10</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="22">
-        <v>2</v>
-      </c>
-      <c r="E15" s="22">
-        <v>2</v>
-      </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="21">
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="11">
         <v>10</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="11">
+        <v>10</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="22">
-        <v>2</v>
-      </c>
-      <c r="E16" s="22">
-        <v>2</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="21">
+      <c r="D18" s="12">
+        <v>2</v>
+      </c>
+      <c r="E18" s="12">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="11">
+        <v>11</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="12">
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="11">
+        <v>12</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="12">
+        <v>2</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="11">
+        <v>13</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" s="12">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="11">
+        <v>16</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="12">
+        <v>2</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="11">
+        <v>17</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="12">
+        <v>2</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="11">
+        <v>18</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12">
+        <v>1</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="14">
+        <v>19</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13">
+        <v>2</v>
+      </c>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="5">
+        <f>SUM(D6:D25)</f>
+        <v>42</v>
+      </c>
+      <c r="E26" s="6">
+        <f>D26-SUM(E6:E25)</f>
+        <v>26</v>
+      </c>
+      <c r="F26" s="6">
+        <f t="shared" ref="F26:I26" si="0">E26-SUM(F6:F25)</f>
+        <v>19</v>
+      </c>
+      <c r="G26" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H26" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I26" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="22">
-        <v>2</v>
-      </c>
-      <c r="E17" s="22">
-        <v>2</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="21">
-        <v>10</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="22">
-        <v>2</v>
-      </c>
-      <c r="E18" s="22">
-        <v>2</v>
-      </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="21">
-        <v>11</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="22">
-        <v>1</v>
-      </c>
-      <c r="E19" s="22">
-        <v>1</v>
-      </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="21">
-        <v>12</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="22">
-        <v>2</v>
-      </c>
-      <c r="E20" s="22">
-        <v>2</v>
-      </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="21">
-        <v>13</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="22">
-        <v>1</v>
-      </c>
-      <c r="E21" s="22">
-        <v>1</v>
-      </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="21">
-        <v>16</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="22">
-        <v>2</v>
-      </c>
-      <c r="E22" s="22">
-        <v>2</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="11">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="11">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="12">
-        <v>2</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="6">
+      <c r="C27" s="19"/>
+      <c r="D27" s="3">
         <f>SUM(D6:D25)</f>
-        <v>40</v>
-      </c>
-      <c r="E26" s="7">
-        <f>D26-SUM(E6:E25)</f>
-        <v>24</v>
-      </c>
-      <c r="F26" s="7">
-        <f t="shared" ref="F26:I26" si="0">E26-SUM(F6:F25)</f>
-        <v>17</v>
-      </c>
-      <c r="G26" s="7">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="H26" s="7">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="I26" s="7">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="4">
-        <f>SUM(D6:D25)</f>
-        <v>40</v>
-      </c>
-      <c r="E27" s="5">
+        <v>42</v>
+      </c>
+      <c r="E27" s="4">
         <f>$D$27-($D$27/5*1)</f>
-        <v>32</v>
-      </c>
-      <c r="F27" s="5">
+        <v>33.6</v>
+      </c>
+      <c r="F27" s="4">
         <f>$D$27-($D$27/5*2)</f>
-        <v>24</v>
-      </c>
-      <c r="G27" s="5">
+        <v>25.2</v>
+      </c>
+      <c r="G27" s="4">
         <f>$D$27-($D$27/5*3)</f>
-        <v>16</v>
-      </c>
-      <c r="H27" s="5">
+        <v>16.799999999999997</v>
+      </c>
+      <c r="H27" s="4">
         <f>$D$27-($D$27/5*4)</f>
-        <v>8</v>
-      </c>
-      <c r="I27" s="5">
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="I27" s="4">
         <f>$D$27-($D$27/5*5)</f>
         <v>0</v>
       </c>

</xml_diff>